<commit_message>
adding excel formating and vaidations
</commit_message>
<xml_diff>
--- a/sdm_test_suite.xlsx
+++ b/sdm_test_suite.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="SMOKE" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="INSTRUCTIONS" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="REFERENCE" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,6 +30,23 @@
     <font>
       <b val="1"/>
       <color rgb="00FFFFFF"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00366092"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00D63384"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00D63384"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -80,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -89,6 +108,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -461,7 +485,7 @@
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
@@ -1004,7 +1028,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="10">
     <dataValidation sqref="A2:A100" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="Invalid Value" error="Please select TRUE or FALSE" type="list">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
@@ -1014,7 +1038,639 @@
     <dataValidation sqref="H2:H100" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="Invalid Result" error="Please select PASS, FAIL, or SKIP" type="list">
       <formula1>"PASS,FAIL,SKIP"</formula1>
     </dataValidation>
+    <dataValidation sqref="A2:A1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Input" error="Invalid value for Enable" promptTitle="Select Enable" prompt="Please select from: TRUE, FALSE" type="list">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Input" error="Invalid value for Application_Name" promptTitle="Select Application_Name" prompt="Please select from: POSTGRES, DUMMY, DATABASE, MYAPP" type="list">
+      <formula1>"POSTGRES,DUMMY,DATABASE,MYAPP"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Input" error="Invalid value for Environment_Name" promptTitle="Select Environment_Name" prompt="Please select from: TEST, UAT, DEV, PROD, STAGING" type="list">
+      <formula1>"TEST,UAT,DEV,PROD,STAGING"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Input" error="Invalid value for Priority" promptTitle="Select Priority" prompt="Please select from: LOW, HIGH, MEDIUM" type="list">
+      <formula1>"LOW,HIGH,MEDIUM"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Input" error="Invalid value for Test_Category" promptTitle="Select Test_Category" prompt="Please select from: SETUP, CONFIGURATION, SECURITY, CONNECTION, QUERIES, PERFORMANCE, COMPATIBILITY, MONITORING, BACKUP" type="list">
+      <formula1>"SETUP,CONFIGURATION,SECURITY,CONNECTION,QUERIES,PERFORMANCE,COMPATIBILITY,MONITORING,BACKUP"</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2:H1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Input" error="Invalid value for Expected_Result" promptTitle="Select Expected_Result" prompt="Please select from: FAIL, SKIP, PASS" type="list">
+      <formula1>"FAIL,SKIP,PASS"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I2:I1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Timeout" error="Timeout must be between 5 and 3600 seconds" promptTitle="Timeout Seconds" prompt="Enter timeout in seconds (5-3600)" type="whole" operator="between">
+      <formula1>5</formula1>
+      <formula2>3600</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="80" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>📋 Excel Test Suite Instructions</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>🎯 HOW TO USE THIS TEMPLATE:</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1. Use the 'SMOKE' worksheet to define your test cases</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2. Fill in each row with test case details</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>3. Use DROPDOWNS for columns with validation (they have blue headers)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>4. Required fields are marked with * in the reference sheet</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>📝 IMPORTANT NOTES:</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>• Test_Case_ID must be unique (e.g., SMOKE_PG_001, SMOKE_PG_002)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>• Test_Category determines which test function will be executed</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>• Use dropdowns to prevent data entry errors</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>• Timeout_Seconds must be between 5-3600 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>• Tags should be comma-separated without spaces</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="inlineStr">
+        <is>
+          <t>🔍 VALIDATION:</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>• Run 'python validate_excel.py' to check for errors</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>• Fix all validation errors before running tests</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>• Use 'python validate_excel.py --fix-suggestions' for help</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="7" t="inlineStr">
+        <is>
+          <t>🚀 EXECUTION:</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>• Run 'python excel_test_driver.py --reports' to execute tests</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>• Use filters like --priority HIGH or --category CONNECTION</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>• Generated reports will be saved in test_reports/ directory</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="7" t="inlineStr">
+        <is>
+          <t>💡 TIPS:</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>• Copy existing rows and modify instead of typing from scratch</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>• Always validate before sharing the file with others</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>• Check the REFERENCE sheet for valid values and mappings</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="40" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="35" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>📚 Test Category Reference &amp; Valid Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="inlineStr">
+        <is>
+          <t>🎯 TEST CATEGORY → FUNCTION MAPPING:</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="9" t="inlineStr">
+        <is>
+          <t>Test_Category</t>
+        </is>
+      </c>
+      <c r="B5" s="9" t="inlineStr">
+        <is>
+          <t>Python Function</t>
+        </is>
+      </c>
+      <c r="C5" s="9" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="D5" s="9" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SETUP</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>test_environment_setup()</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>✅ Available</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Validates environment setup</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>CONFIGURATION</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>test_dummy_config_availability()</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>✅ Available</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Checks configuration availability</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SECURITY</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>test_environment_credentials()</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>✅ Available</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Validates credentials</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>CONNECTION</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>test_postgresql_connection()</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>✅ Available</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Tests database connection</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>QUERIES</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>test_postgresql_basic_queries()</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>✅ Available</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Tests SQL query execution</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>PERFORMANCE</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>test_postgresql_connection_performance()</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>✅ Available</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Tests connection performance</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>COMPATIBILITY</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>test_compatibility()</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>⚠️ Not implemented</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Backwards compatibility testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>MONITORING</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>test_monitoring()</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>🔜 Future</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>System monitoring tests</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>BACKUP</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>test_backup_restore()</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>🔜 Future</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Backup and restore tests</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="8" t="inlineStr">
+        <is>
+          <t>📊 VALID VALUES FOR DROPDOWN FIELDS:</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="inlineStr">
+        <is>
+          <t>Enable:</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>TRUE, FALSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>Priority:</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>LOW, HIGH, MEDIUM</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="10" t="inlineStr">
+        <is>
+          <t>Test_Category:</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SETUP, CONFIGURATION, SECURITY, CONNECTION, QUERIES, PERFORMANCE, COMPATIBILITY, MONITORING, BACKUP</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="10" t="inlineStr">
+        <is>
+          <t>Expected_Result:</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>FAIL, SKIP, PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="10" t="inlineStr">
+        <is>
+          <t>Environment_Name:</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>TEST, UAT, DEV, PROD, STAGING</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="10" t="inlineStr">
+        <is>
+          <t>Application_Name:</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>POSTGRES, DUMMY, DATABASE, MYAPP</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="8" t="inlineStr">
+        <is>
+          <t>⚠️ FIELD REQUIREMENTS:</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>• Test_Case_ID: Must be unique, format: SMOKE_PG_001</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>• Test_Case_Name: Required, descriptive name</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>• Timeout_Seconds: Number between 5-3600</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>• Description: Max 500 characters</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>• Prerequisites: Max 1000 characters</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>• Tags: Comma-separated, no spaces in individual tags</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>